<commit_message>
CooperDI HW Yellow area
</commit_message>
<xml_diff>
--- a/53_mock_ege_test/18.xlsx
+++ b/53_mock_ege_test/18.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub repos\ICT_EGE\53_mock_ege_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A48B77-FF0D-4BBF-A0C4-11A6C635B744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FCDFF4-AD08-4178-8986-0D2C4ADC7AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-6000" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Команды</t>
   </si>
@@ -56,12 +56,21 @@
   <si>
     <t>в таком порядке</t>
   </si>
+  <si>
+    <t>Посетив клетку, Робот забирает монету с собой в том случае, если её значение четно, если в клетке лежит монета нечетного достоинства, Робот не берет из клетки ничего; это также относится к начальной и конечной клетке маршрута Робота.</t>
+  </si>
+  <si>
+    <t>Не учёл условие!! Сразу пошёл решать!!</t>
+  </si>
+  <si>
+    <t>Исп. Фунцию ОСТАТ</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +82,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -195,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -207,6 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -239,8 +257,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>111038</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="2" name="Рукописный ввод 1">
@@ -259,7 +277,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="2" name="Рукописный ввод 1">
@@ -304,8 +322,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>147780</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="3" name="Рукописный ввод 2">
@@ -324,7 +342,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="3" name="Рукописный ввод 2">
@@ -678,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8:N9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,6 +740,9 @@
       <c r="K1" s="3">
         <v>59</v>
       </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
@@ -757,6 +778,9 @@
       <c r="K2" s="5">
         <v>21</v>
       </c>
+      <c r="M2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -1102,509 +1126,515 @@
         <v>716</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <f>MIN(B13,A14)+A1</f>
-        <v>716</v>
+    <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" ref="A13:A16" si="0">IF(MOD(B2,2)=0,B2,0)+MAX(A14,B13)</f>
+        <v>734</v>
       </c>
       <c r="B13">
-        <f>MIN(C13,B14)+B1</f>
-        <v>668</v>
+        <f t="shared" ref="B13:B16" si="1">IF(MOD(C2,2)=0,C2,0)+MAX(B14,C13)</f>
+        <v>676</v>
       </c>
       <c r="C13">
-        <f>MIN(D13,C14)+C1</f>
-        <v>647</v>
+        <f t="shared" ref="C13:C15" si="2">IF(MOD(D2,2)=0,D2,0)+MAX(C14,D13)</f>
+        <v>666</v>
       </c>
       <c r="D13">
-        <f>MIN(E13,D14)+D1</f>
-        <v>590</v>
+        <f t="shared" ref="D13:D15" si="3">IF(MOD(E2,2)=0,E2,0)+MAX(D14,E13)</f>
+        <v>666</v>
       </c>
       <c r="E13">
-        <f>MIN(F13,E14)+E1</f>
-        <v>541</v>
+        <f t="shared" ref="E13:E15" si="4">IF(MOD(F2,2)=0,F2,0)+MAX(E14,F13)</f>
+        <v>580</v>
       </c>
       <c r="F13">
-        <f>MIN(G13,F14)+F1</f>
-        <v>531</v>
+        <f t="shared" ref="F13:F15" si="5">IF(MOD(G2,2)=0,G2,0)+MAX(F14,G13)</f>
+        <v>546</v>
       </c>
       <c r="G13">
-        <f>MIN(H13,G14)+G1</f>
-        <v>567</v>
+        <f t="shared" ref="G13:G15" si="6">IF(MOD(H2,2)=0,H2,0)+MAX(G14,H13)</f>
+        <v>546</v>
       </c>
       <c r="H13">
-        <f>MIN(I13,H14)+H1</f>
-        <v>475</v>
+        <f t="shared" ref="H13:H15" si="7">IF(MOD(I2,2)=0,I2,0)+MAX(H14,I13)</f>
+        <v>532</v>
       </c>
       <c r="I13">
-        <f>MIN(J13,I14)+I1</f>
-        <v>465</v>
+        <f t="shared" ref="I13:I15" si="8">IF(MOD(J2,2)=0,J2,0)+MAX(I14,J13)</f>
+        <v>388</v>
       </c>
       <c r="J13">
-        <f>MIN(K13,J14)+J1</f>
-        <v>446</v>
-      </c>
-      <c r="K13" s="5">
-        <f t="shared" ref="K13:K21" si="0">K14+K1</f>
-        <v>409</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J13:J17" si="9">IF(MOD(K2,2)=0,K2,0)+MAX(J14,K13)</f>
+        <v>388</v>
+      </c>
+      <c r="K13" s="8">
+        <f t="shared" ref="K13:K21" si="10">IF(MOD(K1,2)=0,K1,0)+K14</f>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f>MIN(B14,A15)+A2</f>
-        <v>731</v>
+        <f t="shared" si="0"/>
+        <v>676</v>
       </c>
       <c r="B14">
-        <f>MIN(C14,B15)+B2</f>
-        <v>788</v>
+        <f t="shared" si="1"/>
+        <v>676</v>
       </c>
       <c r="C14">
-        <f>MIN(D14,C15)+C2</f>
-        <v>746</v>
+        <f t="shared" si="2"/>
+        <v>592</v>
       </c>
       <c r="D14">
-        <f>MIN(E14,D15)+D2</f>
-        <v>649</v>
+        <f t="shared" si="3"/>
+        <v>592</v>
       </c>
       <c r="E14">
-        <f>MIN(F14,E15)+E2</f>
-        <v>581</v>
+        <f t="shared" si="4"/>
+        <v>546</v>
       </c>
       <c r="F14">
-        <f>MIN(G14,F15)+F2</f>
-        <v>507</v>
+        <f t="shared" si="5"/>
+        <v>546</v>
       </c>
       <c r="G14">
-        <f>MIN(H14,G15)+G2</f>
-        <v>473</v>
+        <f t="shared" si="6"/>
+        <v>546</v>
       </c>
       <c r="H14">
-        <f>MIN(I14,H15)+H2</f>
-        <v>460</v>
+        <f t="shared" si="7"/>
+        <v>458</v>
       </c>
       <c r="I14">
-        <f>MIN(J14,I15)+I2</f>
-        <v>439</v>
+        <f t="shared" si="8"/>
+        <v>388</v>
       </c>
       <c r="J14">
-        <f>MIN(K14,J15)+J2</f>
-        <v>382</v>
-      </c>
-      <c r="K14" s="5">
+        <f t="shared" si="9"/>
+        <v>388</v>
+      </c>
+      <c r="K14" s="8">
+        <f t="shared" si="10"/>
+        <v>234</v>
+      </c>
+      <c r="M14">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15">
         <f t="shared" si="0"/>
-        <v>350</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f>MIN(B15,A16)+A3</f>
-        <v>652</v>
+        <v>616</v>
       </c>
       <c r="B15">
-        <f>MIN(C15,B16)+B3</f>
-        <v>730</v>
+        <f t="shared" si="1"/>
+        <v>524</v>
       </c>
       <c r="C15">
-        <f>MIN(D15,C16)+C3</f>
-        <v>652</v>
+        <f t="shared" si="2"/>
+        <v>524</v>
       </c>
       <c r="D15">
-        <f>MIN(E15,D16)+D3</f>
-        <v>568</v>
+        <f t="shared" si="3"/>
+        <v>478</v>
       </c>
       <c r="E15">
-        <f>MIN(F15,E16)+E3</f>
-        <v>529</v>
+        <f t="shared" si="4"/>
+        <v>452</v>
       </c>
       <c r="F15">
-        <f>MIN(G15,F16)+F3</f>
-        <v>483</v>
+        <f t="shared" si="5"/>
+        <v>440</v>
       </c>
       <c r="G15">
-        <f>MIN(H15,G16)+G3</f>
-        <v>462</v>
+        <f t="shared" si="6"/>
+        <v>440</v>
       </c>
       <c r="H15">
-        <f>MIN(I15,H16)+H3</f>
-        <v>453</v>
+        <f t="shared" si="7"/>
+        <v>440</v>
       </c>
       <c r="I15">
-        <f>MIN(J15,I16)+I3</f>
-        <v>365</v>
+        <f t="shared" si="8"/>
+        <v>358</v>
       </c>
       <c r="J15">
-        <f>MIN(K15,J16)+J3</f>
-        <v>347</v>
-      </c>
-      <c r="K15" s="5">
-        <f t="shared" si="0"/>
-        <v>329</v>
+        <f t="shared" si="9"/>
+        <v>358</v>
+      </c>
+      <c r="K15" s="8">
+        <f t="shared" si="10"/>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f>MIN(B16,A17)+A4</f>
-        <v>612</v>
+        <f t="shared" si="0"/>
+        <v>616</v>
       </c>
       <c r="B16">
-        <f>MIN(C16,B17)+B4</f>
-        <v>651</v>
-      </c>
-      <c r="C16" s="10">
-        <f t="shared" ref="C16:H16" si="1">D16+C4</f>
-        <v>591</v>
-      </c>
-      <c r="D16" s="10">
         <f t="shared" si="1"/>
-        <v>540</v>
-      </c>
-      <c r="E16" s="10">
-        <f t="shared" si="1"/>
-        <v>494</v>
-      </c>
-      <c r="F16" s="10">
-        <f t="shared" si="1"/>
-        <v>468</v>
-      </c>
-      <c r="G16" s="10">
-        <f t="shared" si="1"/>
-        <v>456</v>
-      </c>
-      <c r="H16" s="10">
-        <f t="shared" si="1"/>
-        <v>449</v>
-      </c>
-      <c r="I16" s="10">
-        <f>J16+I4</f>
-        <v>358</v>
+        <v>476</v>
+      </c>
+      <c r="C16" s="8">
+        <f t="shared" ref="C16:H16" si="11">IF(MOD(C4,2)=0,C4,0)+D16</f>
+        <v>432</v>
+      </c>
+      <c r="D16" s="8">
+        <f t="shared" si="11"/>
+        <v>432</v>
+      </c>
+      <c r="E16" s="8">
+        <f t="shared" si="11"/>
+        <v>386</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="11"/>
+        <v>360</v>
+      </c>
+      <c r="G16" s="8">
+        <f t="shared" si="11"/>
+        <v>348</v>
+      </c>
+      <c r="H16" s="8">
+        <f t="shared" si="11"/>
+        <v>348</v>
+      </c>
+      <c r="I16" s="8">
+        <f>IF(MOD(I4,2)=0,I4,0)+J16</f>
+        <v>348</v>
       </c>
       <c r="J16">
-        <f>MIN(K16,J17)+J4</f>
-        <v>276</v>
-      </c>
-      <c r="K16" s="5">
-        <f t="shared" si="0"/>
-        <v>299</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>266</v>
+      </c>
+      <c r="K16" s="8">
+        <f t="shared" si="10"/>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17">
-        <f>MIN(B17,A18)+A5</f>
-        <v>602</v>
+        <f t="shared" ref="A17:A22" si="12">IF(MOD(B6,2)=0,B6,0)+MAX(A18,B17)</f>
+        <v>564</v>
       </c>
       <c r="B17">
-        <f>MIN(C17,B18)+B5</f>
-        <v>584</v>
+        <f t="shared" ref="B17:B22" si="13">IF(MOD(C6,2)=0,C6,0)+MAX(B18,C17)</f>
+        <v>476</v>
       </c>
       <c r="C17">
-        <f>MIN(D17,C18)+C5</f>
-        <v>532</v>
+        <f t="shared" ref="C17:C22" si="14">IF(MOD(D6,2)=0,D6,0)+MAX(C18,D17)</f>
+        <v>460</v>
       </c>
       <c r="D17">
-        <f>MIN(E17,D18)+D5</f>
-        <v>547</v>
+        <f t="shared" ref="D17:D22" si="15">IF(MOD(E6,2)=0,E6,0)+MAX(D18,E17)</f>
+        <v>304</v>
       </c>
       <c r="E17">
-        <f>MIN(F17,E18)+E5</f>
-        <v>470</v>
+        <f t="shared" ref="E17:E22" si="16">IF(MOD(F6,2)=0,F6,0)+MAX(E18,F17)</f>
+        <v>252</v>
       </c>
       <c r="F17">
-        <f>MIN(G17,F18)+F5</f>
-        <v>371</v>
+        <f t="shared" ref="F17:F22" si="17">IF(MOD(G6,2)=0,G6,0)+MAX(F18,G17)</f>
+        <v>252</v>
       </c>
       <c r="G17">
-        <f>MIN(H17,G18)+G5</f>
-        <v>419</v>
+        <f t="shared" ref="G17:G22" si="18">IF(MOD(H6,2)=0,H6,0)+MAX(G18,H17)</f>
+        <v>206</v>
       </c>
       <c r="H17">
-        <f>MIN(I17,H18)+H5</f>
-        <v>325</v>
+        <f t="shared" ref="H17:H22" si="19">IF(MOD(I6,2)=0,I6,0)+MAX(H18,I17)</f>
+        <v>206</v>
       </c>
       <c r="I17">
-        <f>MIN(J17,I18)+I5</f>
-        <v>266</v>
+        <f t="shared" ref="I17:I22" si="20">IF(MOD(J6,2)=0,J6,0)+MAX(I18,J17)</f>
+        <v>122</v>
       </c>
       <c r="J17">
-        <f>MIN(K17,J18)+J5</f>
-        <v>249</v>
-      </c>
-      <c r="K17" s="5">
-        <f t="shared" si="0"/>
-        <v>207</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>122</v>
+      </c>
+      <c r="K17" s="8">
+        <f t="shared" si="10"/>
+        <v>112</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f>MIN(B18,A19)+A6</f>
-        <v>575</v>
+        <f t="shared" si="12"/>
+        <v>448</v>
       </c>
       <c r="B18">
-        <f>MIN(C18,B19)+B6</f>
-        <v>533</v>
+        <f t="shared" si="13"/>
+        <v>364</v>
       </c>
       <c r="C18">
-        <f>MIN(D18,C19)+C6</f>
-        <v>445</v>
+        <f t="shared" si="14"/>
+        <v>364</v>
       </c>
       <c r="D18">
-        <f>MIN(E18,D19)+D6</f>
-        <v>487</v>
+        <f t="shared" si="15"/>
+        <v>304</v>
       </c>
       <c r="E18">
-        <f>MIN(F18,E19)+E6</f>
-        <v>422</v>
+        <f t="shared" si="16"/>
+        <v>252</v>
       </c>
       <c r="F18">
-        <f>MIN(G18,F19)+F6</f>
-        <v>353</v>
+        <f t="shared" si="17"/>
+        <v>252</v>
       </c>
       <c r="G18">
-        <f>MIN(H18,G19)+G6</f>
-        <v>325</v>
+        <f t="shared" si="18"/>
+        <v>172</v>
       </c>
       <c r="H18">
-        <f>MIN(I18,H19)+H6</f>
-        <v>240</v>
+        <f t="shared" si="19"/>
+        <v>90</v>
       </c>
       <c r="I18">
-        <f>MIN(J18,I19)+I6</f>
+        <f t="shared" si="20"/>
+        <v>80</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ref="J17:J21" si="21">IF(MOD(K7,2)=0,K7,0)+MAX(J19,K18)</f>
+        <v>80</v>
+      </c>
+      <c r="K18" s="8">
+        <f t="shared" si="10"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="12"/>
+        <v>386</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="13"/>
+        <v>312</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="14"/>
+        <v>242</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="15"/>
+        <v>206</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="16"/>
+        <v>206</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="17"/>
+        <v>144</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="18"/>
+        <v>134</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="19"/>
+        <v>90</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="20"/>
+        <v>80</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="21"/>
+        <v>80</v>
+      </c>
+      <c r="K19" s="8">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="12"/>
+        <v>386</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="13"/>
+        <v>312</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="14"/>
+        <v>242</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="15"/>
+        <v>154</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="16"/>
+        <v>136</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="17"/>
+        <v>136</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="18"/>
+        <v>116</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="19"/>
+        <v>80</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="20"/>
+        <v>80</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="21"/>
+        <v>80</v>
+      </c>
+      <c r="K20" s="8">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="12"/>
         <v>286</v>
       </c>
-      <c r="J18">
-        <f>MIN(K18,J19)+J6</f>
-        <v>214</v>
-      </c>
-      <c r="K18" s="5">
-        <f t="shared" si="0"/>
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f>MIN(B19,A20)+A7</f>
-        <v>494</v>
-      </c>
-      <c r="B19">
-        <f>MIN(C19,B20)+B7</f>
-        <v>487</v>
-      </c>
-      <c r="C19">
-        <f>MIN(D19,C20)+C7</f>
-        <v>429</v>
-      </c>
-      <c r="D19">
-        <f>MIN(E19,D20)+D7</f>
-        <v>391</v>
-      </c>
-      <c r="E19">
-        <f>MIN(F19,E20)+E7</f>
-        <v>354</v>
-      </c>
-      <c r="F19">
-        <f>MIN(G19,F20)+F7</f>
-        <v>308</v>
-      </c>
-      <c r="G19">
-        <f>MIN(H19,G20)+G7</f>
-        <v>241</v>
-      </c>
-      <c r="H19">
-        <f>MIN(I19,H20)+H7</f>
-        <v>191</v>
-      </c>
-      <c r="I19">
-        <f>MIN(J19,I20)+I7</f>
-        <v>202</v>
-      </c>
-      <c r="J19">
-        <f>MIN(K19,J20)+J7</f>
-        <v>166</v>
-      </c>
-      <c r="K19" s="5">
-        <f t="shared" si="0"/>
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f>MIN(B20,A21)+A8</f>
-        <v>499</v>
-      </c>
-      <c r="B20">
-        <f>MIN(C20,B21)+B8</f>
-        <v>425</v>
-      </c>
-      <c r="C20">
-        <f>MIN(D20,C21)+C8</f>
-        <v>368</v>
-      </c>
-      <c r="D20">
-        <f>MIN(E20,D21)+D8</f>
-        <v>331</v>
-      </c>
-      <c r="E20">
-        <f>MIN(F20,E21)+E8</f>
-        <v>302</v>
-      </c>
-      <c r="F20">
-        <f>MIN(G20,F21)+F8</f>
-        <v>223</v>
-      </c>
-      <c r="G20">
-        <f>MIN(H20,G21)+G8</f>
-        <v>161</v>
-      </c>
-      <c r="H20">
-        <f>MIN(I20,H21)+H8</f>
-        <v>153</v>
-      </c>
-      <c r="I20">
-        <f>MIN(J20,I21)+I8</f>
-        <v>135</v>
-      </c>
-      <c r="J20">
-        <f>MIN(K20,J21)+J8</f>
-        <v>149</v>
-      </c>
-      <c r="K20" s="5">
-        <f t="shared" si="0"/>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f>MIN(B21,A22)+A9</f>
-        <v>515</v>
-      </c>
       <c r="B21">
-        <f>MIN(C21,B22)+B9</f>
-        <v>442</v>
+        <f t="shared" si="13"/>
+        <v>286</v>
       </c>
       <c r="C21">
-        <f>MIN(D21,C22)+C9</f>
-        <v>368</v>
+        <f t="shared" si="14"/>
+        <v>142</v>
       </c>
       <c r="D21">
-        <f>MIN(E21,D22)+D9</f>
-        <v>342</v>
+        <f t="shared" si="15"/>
+        <v>120</v>
       </c>
       <c r="E21">
-        <f>MIN(F21,E22)+E9</f>
-        <v>254</v>
+        <f t="shared" si="16"/>
+        <v>120</v>
       </c>
       <c r="F21">
-        <f>MIN(G21,F22)+F9</f>
-        <v>236</v>
+        <f t="shared" si="17"/>
+        <v>86</v>
       </c>
       <c r="G21">
-        <f>MIN(H21,G22)+G9</f>
-        <v>181</v>
+        <f t="shared" si="18"/>
+        <v>80</v>
       </c>
       <c r="H21">
-        <f>MIN(I21,H22)+H9</f>
-        <v>161</v>
+        <f t="shared" si="19"/>
+        <v>80</v>
       </c>
       <c r="I21">
-        <f>MIN(J21,I22)+I9</f>
-        <v>125</v>
+        <f t="shared" si="20"/>
+        <v>80</v>
       </c>
       <c r="J21">
-        <f>MIN(K21,J22)+J9</f>
-        <v>82</v>
-      </c>
-      <c r="K21" s="5">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="21"/>
+        <v>80</v>
+      </c>
+      <c r="K21" s="8">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f>MIN(B22,A23)+A10</f>
-        <v>543</v>
+        <f t="shared" si="12"/>
+        <v>220</v>
       </c>
       <c r="B22">
-        <f>MIN(C22,B23)+B10</f>
-        <v>529</v>
+        <f t="shared" si="13"/>
+        <v>206</v>
       </c>
       <c r="C22">
-        <f>MIN(D22,C23)+C10</f>
-        <v>494</v>
+        <f t="shared" si="14"/>
+        <v>142</v>
       </c>
       <c r="D22">
-        <f>MIN(E22,D23)+D10</f>
-        <v>414</v>
+        <f t="shared" si="15"/>
+        <v>120</v>
       </c>
       <c r="E22">
-        <f>MIN(F22,E23)+E10</f>
-        <v>389</v>
+        <f t="shared" si="16"/>
+        <v>120</v>
       </c>
       <c r="F22">
-        <f>MIN(G22,F23)+F10</f>
-        <v>314</v>
+        <f t="shared" si="17"/>
+        <v>78</v>
       </c>
       <c r="G22">
-        <f>MIN(H22,G23)+G10</f>
-        <v>219</v>
+        <f t="shared" si="18"/>
+        <v>76</v>
       </c>
       <c r="H22">
-        <f>MIN(I22,H23)+H10</f>
-        <v>249</v>
+        <f t="shared" si="19"/>
+        <v>60</v>
       </c>
       <c r="I22">
-        <f>MIN(J22,I23)+I10</f>
-        <v>206</v>
+        <f t="shared" si="20"/>
+        <v>60</v>
       </c>
       <c r="J22">
-        <f>MIN(K22,J23)+J10</f>
-        <v>111</v>
-      </c>
-      <c r="K22" s="5">
-        <f>K23+K10</f>
+        <f>IF(MOD(K11,2)=0,K11,0)+MAX(J23,K22)</f>
+        <v>60</v>
+      </c>
+      <c r="K22" s="8">
+        <f>IF(MOD(K10,2)=0,K10,0)+K23</f>
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
-        <f t="shared" ref="A23:I23" si="2">B23+A11</f>
-        <v>600</v>
-      </c>
-      <c r="B23" s="7">
-        <f t="shared" si="2"/>
-        <v>522</v>
-      </c>
-      <c r="C23" s="7">
-        <f t="shared" si="2"/>
-        <v>499</v>
-      </c>
-      <c r="D23" s="7">
-        <f t="shared" si="2"/>
-        <v>435</v>
-      </c>
-      <c r="E23" s="7">
-        <f t="shared" si="2"/>
-        <v>344</v>
-      </c>
-      <c r="F23" s="7">
-        <f t="shared" si="2"/>
-        <v>255</v>
-      </c>
-      <c r="G23" s="7">
-        <f t="shared" si="2"/>
-        <v>213</v>
-      </c>
-      <c r="H23" s="7">
-        <f t="shared" si="2"/>
-        <v>150</v>
-      </c>
-      <c r="I23" s="7">
-        <f t="shared" si="2"/>
-        <v>134</v>
-      </c>
-      <c r="J23" s="7">
-        <f>K23+J11</f>
-        <v>107</v>
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <f t="shared" ref="A23:I23" si="22">IF(MOD(A11,2)=0,A11,0)+B23</f>
+        <v>220</v>
+      </c>
+      <c r="B23" s="8">
+        <f t="shared" si="22"/>
+        <v>142</v>
+      </c>
+      <c r="C23" s="8">
+        <f t="shared" si="22"/>
+        <v>142</v>
+      </c>
+      <c r="D23" s="8">
+        <f t="shared" si="22"/>
+        <v>78</v>
+      </c>
+      <c r="E23" s="8">
+        <f t="shared" si="22"/>
+        <v>78</v>
+      </c>
+      <c r="F23" s="8">
+        <f t="shared" si="22"/>
+        <v>78</v>
+      </c>
+      <c r="G23" s="8">
+        <f t="shared" si="22"/>
+        <v>36</v>
+      </c>
+      <c r="H23" s="8">
+        <f t="shared" si="22"/>
+        <v>36</v>
+      </c>
+      <c r="I23" s="8">
+        <f t="shared" si="22"/>
+        <v>20</v>
+      </c>
+      <c r="J23" s="8">
+        <f>IF(MOD(J11,2)=0,J11,0)+K23</f>
+        <v>20</v>
       </c>
       <c r="K23" s="8">
-        <f>K11</f>
+        <f>IF(MOD(K11,2)=0,K11,0)</f>
         <v>20</v>
       </c>
     </row>

</xml_diff>